<commit_message>
update from office computer
</commit_message>
<xml_diff>
--- a/Data/Modeling/BHE_Data_v2.xlsx
+++ b/Data/Modeling/BHE_Data_v2.xlsx
@@ -15,7 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="196">
   <si>
     <t>average energy consumption for a household</t>
   </si>
@@ -482,9 +483,6 @@
     <t>hot water heating</t>
   </si>
   <si>
-    <t>gas consumption</t>
-  </si>
-  <si>
     <t>average yearly (kWh)</t>
   </si>
   <si>
@@ -565,12 +563,66 @@
   <si>
     <t xml:space="preserve">cyclical + recharge required </t>
   </si>
+  <si>
+    <t>w/m2</t>
+  </si>
+  <si>
+    <t>kwh/d</t>
+  </si>
+  <si>
+    <t>kwh/y</t>
+  </si>
+  <si>
+    <t>average annual rate</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>J solar in 1 year</t>
+  </si>
+  <si>
+    <t>KWh solar</t>
+  </si>
+  <si>
+    <t>J consummed</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>W/m²</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>mined</t>
+  </si>
+  <si>
+    <t>heating requirements</t>
+  </si>
+  <si>
+    <t>rho_r</t>
+  </si>
+  <si>
+    <t>c_r</t>
+  </si>
+  <si>
+    <t>rho_w</t>
+  </si>
+  <si>
+    <t>c_w</t>
+  </si>
+  <si>
+    <t>m²</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,8 +646,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,6 +676,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -665,6 +730,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,6 +793,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3219,6 +3291,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7742,6 +7815,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -7827,6 +7901,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -7873,6 +7948,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8783,17 +8859,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
@@ -8815,7 +8893,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>12400</v>
+        <v>15000</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -8848,7 +8926,7 @@
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3">
         <f>B2*1000*3600</f>
-        <v>44640000000</v>
+        <v>54000000000</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -8877,7 +8955,7 @@
       </c>
       <c r="B4">
         <f>B3/(365*24*3600)</f>
-        <v>1415.5251141552512</v>
+        <v>1712.3287671232877</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -8918,7 +8996,7 @@
       </c>
       <c r="B5">
         <f>B4/2.25</f>
-        <v>629.12227295788944</v>
+        <v>761.03500761035002</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
@@ -8973,7 +9051,7 @@
       </c>
       <c r="B7">
         <f>B4/B6</f>
-        <v>416.33091592801509</v>
+        <v>503.62610797743758</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -9137,34 +9215,34 @@
       </c>
       <c r="C16">
         <f>B4-B4/B6</f>
-        <v>999.19419822723614</v>
+        <v>1208.70265914585</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17">
         <f>C16+B7</f>
-        <v>1415.5251141552512</v>
+        <v>1712.3287671232877</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>68</v>
       </c>
       <c r="C18">
         <f>C16/5</f>
-        <v>199.83883964544722</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+        <v>241.74053182917001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -9175,7 +9253,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -9186,13 +9264,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>49</v>
       </c>
       <c r="B22">
         <f>C16/(120-40)</f>
-        <v>12.489927477840451</v>
+        <v>15.108783239323126</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
@@ -9201,10 +9279,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23">
         <f>C16/(80-40)</f>
-        <v>24.979854955680903</v>
+        <v>30.217566478646251</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
@@ -9213,41 +9291,45 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="R29">
-        <f>25*40</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>144</v>
       </c>
       <c r="C36" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F36" s="15">
+        <v>8</v>
+      </c>
+      <c r="G36" s="15">
+        <v>8</v>
+      </c>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>143</v>
       </c>
@@ -9257,8 +9339,17 @@
       <c r="C37">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F37" s="15">
+        <f>F36*70</f>
+        <v>560</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>146</v>
       </c>
@@ -9272,8 +9363,18 @@
       <c r="D38" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F38" s="15">
+        <v>1380</v>
+      </c>
+      <c r="G38" s="15">
+        <v>1380</v>
+      </c>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C39">
         <f>C38*3600*1000</f>
         <v>5040000000</v>
@@ -9281,8 +9382,20 @@
       <c r="D39" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F39" s="15">
+        <f>F38*3600</f>
+        <v>4968000</v>
+      </c>
+      <c r="G39" s="15">
+        <f>G38*3600</f>
+        <v>4968000</v>
+      </c>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C40">
         <f>C39/(365.25*86400)</f>
         <v>159.7079625827059</v>
@@ -9290,12 +9403,251 @@
       <c r="D40" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F40" s="15">
+        <f>F37*F39</f>
+        <v>2782080000</v>
+      </c>
+      <c r="G40" s="15">
+        <f>G36*G39</f>
+        <v>39744000</v>
+      </c>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C41">
         <f>C37*3600*1000/86400</f>
         <v>145.83333333333334</v>
       </c>
+      <c r="F41" s="15">
+        <v>772</v>
+      </c>
+      <c r="G41" s="15">
+        <v>11</v>
+      </c>
+      <c r="H41" s="15">
+        <f>F41/70</f>
+        <v>11.028571428571428</v>
+      </c>
+      <c r="I41" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F42" s="16">
+        <v>31500000000</v>
+      </c>
+      <c r="G42" s="16">
+        <v>31500000000</v>
+      </c>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>181</v>
+      </c>
+      <c r="F43" s="16">
+        <f>F40/F42*100</f>
+        <v>8.831999999999999</v>
+      </c>
+      <c r="G43" s="16">
+        <f>G40/G42*100</f>
+        <v>0.12617142857142857</v>
+      </c>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>94</v>
+      </c>
+      <c r="C44" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <f>B44/B45</f>
+        <v>11.75</v>
+      </c>
+      <c r="F46">
+        <v>11.5</v>
+      </c>
+      <c r="G46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <f>F46*70</f>
+        <v>805</v>
+      </c>
+      <c r="G47" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>2.5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>179</v>
+      </c>
+      <c r="F48">
+        <f>1380*3600</f>
+        <v>4968000</v>
+      </c>
+      <c r="G48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <f>B48*365</f>
+        <v>912.5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>180</v>
+      </c>
+      <c r="F49" s="18">
+        <f>F47*F48</f>
+        <v>3999240000</v>
+      </c>
+      <c r="G49" s="18">
+        <f>F49/F50*100</f>
+        <v>12.681506849315069</v>
+      </c>
+      <c r="H49" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I49" s="17"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <f>B49*1000*3600</f>
+        <v>3285000000</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="17">
+        <f>1000*365*86400</f>
+        <v>31536000000</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I50" s="17"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <f>B50/(365.25*24*3600)</f>
+        <v>104.0953684690851</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="18">
+        <f>0.068*70*86400*365</f>
+        <v>150111360.00000003</v>
+      </c>
+      <c r="G51" s="18">
+        <f>F51/F50*100</f>
+        <v>0.47600000000000015</v>
+      </c>
+      <c r="H51" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="I51" s="17"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F52" s="18">
+        <f>F50-F49-F51</f>
+        <v>27386648640</v>
+      </c>
+      <c r="G52" s="18">
+        <f>F52/F50*100</f>
+        <v>86.84249315068493</v>
+      </c>
+      <c r="H52" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="I52" s="17"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F53" s="17"/>
+      <c r="G53" s="18">
+        <f>(G52/100*1000)/(40*30)</f>
+        <v>0.72368744292237441</v>
+      </c>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F54" s="17"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F55" s="17"/>
+      <c r="G55" s="17">
+        <v>11.5</v>
+      </c>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F56" s="17"/>
+      <c r="G56" s="17">
+        <f>(1380*3600)/(366*86400)*G55</f>
+        <v>1.8066939890710383</v>
+      </c>
+      <c r="H56" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="I56" s="17"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F57" s="17"/>
+      <c r="G57" s="17">
+        <f>G55*70*1380*3600</f>
+        <v>3999240000</v>
+      </c>
+      <c r="H57" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="I57" s="17"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F58" s="17"/>
+      <c r="G58" s="17">
+        <f>G56*70*366*86400</f>
+        <v>3999240000</v>
+      </c>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9332,7 +9684,7 @@
         <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L1" t="s">
         <v>60</v>
@@ -17088,8 +17440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17906,29 +18258,1070 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="12" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="9.109375" style="17"/>
+    <col min="9" max="9" width="7" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="17">
+        <v>2500</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="17">
+        <v>2500</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="17">
+        <v>950</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="17">
+        <v>950</v>
+      </c>
+      <c r="M2" s="17">
+        <v>1000</v>
+      </c>
+      <c r="N2" s="17">
+        <v>6800</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="7">
+        <f>I7/(I4*I6*I1*I2 * (1-I5))</f>
+        <v>6803.5896192093132</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="17">
+        <v>1415</v>
+      </c>
+      <c r="N3" s="17">
+        <v>9600</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="17">
+        <v>4680</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="17">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="17">
+        <v>5</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="17">
+        <f>I4*I6</f>
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="17">
+        <v>15000</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="17">
+        <f>(40-9)/1000</f>
+        <v>3.1E-2</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="17">
+        <f>B6*3600*1000</f>
+        <v>54000000000</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="9">
+        <f>M2*3600*24*365.25</f>
+        <v>31557600000</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="17">
+        <f>B7/(365*24*3600)</f>
+        <v>1712.3287671232877</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="17">
+        <f>I7*30</f>
+        <v>946728000000</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="17">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="17">
+        <f>B8*(1-1/B9)</f>
+        <v>1208.70265914585</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="8">
+        <v>5</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="18">
+        <v>31500000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="17">
+        <f>B10*24*365.25*3600</f>
+        <v>38143755036.261078</v>
+      </c>
+      <c r="C11" s="17">
+        <f>B11*30</f>
+        <v>1144312651087.8323</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="10">
+        <f>I8/(I10*I1*I2*(1-I5))</f>
+        <v>88582.736842105267</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="O11" s="18">
+        <f>70*0.031</f>
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="O12" s="18">
+        <f>950*2500</f>
+        <v>2375000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="3">
+        <f>B11/(B5*((1-B12)*B1*B2+B12*B3*B4))</f>
+        <v>2927.9412808490561</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="N13" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="13">
+        <f>O10/(O11*O12)</f>
+        <v>6112.0543293718165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="3">
+        <f>(B11*30)/(B5*((1-B12)*B1*B2+B12*B3*B4))</f>
+        <v>87838.238425471674</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="17">
+        <v>40</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="O14" s="18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="6">
+        <f>SQRT(I3/(I14*PI()))</f>
+        <v>7.3580735205142798</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I16" s="8">
+        <f>SQRT(I11/(I14*PI()))</f>
+        <v>26.550311147922169</v>
+      </c>
+      <c r="K16" s="17">
+        <v>6.4736000000000002E-2</v>
+      </c>
+      <c r="L16" s="17">
+        <f>K16*I18</f>
+        <v>143.36230130526314</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="O16" s="17">
+        <f>SQRT(O13/(PI()*O14))</f>
+        <v>6.9741080396196331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="17">
+        <v>40</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="6">
+        <f>I15^2*PI()</f>
+        <v>170.08974048023282</v>
+      </c>
+      <c r="L17" s="17">
+        <f>B10-L16</f>
+        <v>1065.3403578405869</v>
+      </c>
+      <c r="N17" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" s="17">
+        <f>O16^2*PI()</f>
+        <v>152.80135823429541</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="17">
+        <f>SQRT(B13/(B17*PI()))</f>
+        <v>4.8269883360639207</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" s="8">
+        <f>I16^2*PI()</f>
+        <v>2214.5684210526315</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="L18" s="17">
+        <f>L17/(B17)</f>
+        <v>26.633508946014672</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="17">
+        <f>SQRT(B14/(B17*PI()))</f>
+        <v>26.438503964765367</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="L19" s="17">
+        <f>2*PI()*I16</f>
+        <v>166.82052490567094</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="3">
+        <f>PI()*B18^2</f>
+        <v>73.198532021226413</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="11">
+        <f>1000/(K23+K24)</f>
+        <v>5821.5350223546939</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="L20" s="17">
+        <f>L18/L19</f>
+        <v>0.15965366948146612</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="3">
+        <f>PI()*B19^2</f>
+        <v>2195.955960636792</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="6">
+        <f>I17</f>
+        <v>170.08974048023282</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="I22" s="17">
+        <f>I20/I21</f>
+        <v>34.226256127607243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K23" s="11">
+        <f>0.091923</f>
+        <v>9.1923000000000005E-2</v>
+      </c>
+      <c r="L23" s="17">
+        <f>I18*K23</f>
+        <v>203.56977296842106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K24" s="11">
+        <f>K23-0.01207</f>
+        <v>7.9853000000000007E-2</v>
+      </c>
+      <c r="L24" s="17">
+        <f>I18*K24</f>
+        <v>176.8399321263158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="17">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="K25" s="17">
+        <f>K24-K23</f>
+        <v>-1.2069999999999997E-2</v>
+      </c>
+      <c r="L25" s="17">
+        <f>1000-(L23+L24)</f>
+        <v>619.59029490526314</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="17">
+        <f>11.5*(1380*3600)/(365*86400)</f>
+        <v>1.8116438356164384</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="L26" s="8">
+        <f>2*PI()*I16</f>
+        <v>166.82052490567094</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="3">
+        <f>B10/(B25+B26)</f>
+        <v>644.76389390968916</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F27" s="17">
+        <f>75*(1-1/3.4)</f>
+        <v>52.941176470588232</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="L27" s="17">
+        <f>L25/I14</f>
+        <v>15.489757372631578</v>
+      </c>
+      <c r="O27" s="17">
+        <f>0.031*150+9</f>
+        <v>13.65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L28" s="17">
+        <f>L27/L26</f>
+        <v>9.2852827200911273E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="17">
+        <f>B20</f>
+        <v>73.198532021226413</v>
+      </c>
+      <c r="C31" s="17">
+        <f>B21</f>
+        <v>2195.955960636792</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="17">
+        <f>B10</f>
+        <v>1208.70265914585</v>
+      </c>
+      <c r="C32" s="17">
+        <f>B32</f>
+        <v>1208.70265914585</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="19">
+        <v>70</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="17">
+        <f>0.063*B31</f>
+        <v>4.6115075173372642</v>
+      </c>
+      <c r="C33" s="17">
+        <f>B25*C31</f>
+        <v>138.34522552011791</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="19">
+        <f>0.064736*F32</f>
+        <v>4.5315200000000004</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="17">
+        <f>B33*365.25*86400</f>
+        <v>145528109.62912244</v>
+      </c>
+      <c r="C34" s="17">
+        <f>C33*365.25*86400</f>
+        <v>4365843288.8736725</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="19">
+        <v>1000</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="17">
+        <f>B34/B11*100</f>
+        <v>0.3815253886010363</v>
+      </c>
+      <c r="C35" s="17">
+        <f>C34/C11*100</f>
+        <v>0.3815253886010363</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="19">
+        <v>5</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19">
+        <f>F34-F33</f>
+        <v>995.46848</v>
+      </c>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B37" s="17">
+        <f>1200-B33</f>
+        <v>1195.3884924826627</v>
+      </c>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B38" s="17">
+        <f>B37/(40*30)</f>
+        <v>0.99615707706888557</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="17">
+        <f>B38/B25</f>
+        <v>15.812017096331516</v>
+      </c>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="17">
+        <f>B26*B31</f>
+        <v>132.60966931242731</v>
+      </c>
+      <c r="C41" s="17">
+        <f>C31*B26</f>
+        <v>3978.2900793728186</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19">
+        <f>I36/(B46*B17)</f>
+        <v>0.82056200602593243</v>
+      </c>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B42" s="17">
+        <f>B41*365.25*86400</f>
+        <v>4184842900.2938561</v>
+      </c>
+      <c r="C42" s="17">
+        <f>C41*365.25*86400</f>
+        <v>125545287008.81566</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B43" s="17">
+        <f>B42/B11*100</f>
+        <v>10.971239974448153</v>
+      </c>
+      <c r="C43" s="17">
+        <f>C42/C11*100</f>
+        <v>10.971239974448151</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19">
+        <f>F33/F34*100</f>
+        <v>0.45315200000000005</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="3">
+        <f>B32-B33-B41</f>
+        <v>1071.4814823160855</v>
+      </c>
+      <c r="C44" s="3">
+        <f>C32-C33-C41</f>
+        <v>-2907.9326457470866</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19">
+        <f>F34-F46-F47</f>
+        <v>987.95999999999992</v>
+      </c>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="17">
+        <f>B44/B17</f>
+        <v>26.787037057902136</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19">
+        <f>I44/(B46*B17)</f>
+        <v>0.81437278604077967</v>
+      </c>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="17">
+        <f>2*PI()*B18</f>
+        <v>30.328862191084067</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="19">
+        <f>0.092*70</f>
+        <v>6.4399999999999995</v>
+      </c>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="17">
+        <f>B45/B46</f>
+        <v>0.88321932056445096</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F47" s="19">
+        <f>0.08*70</f>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B48" s="17">
+        <f>B47/B25</f>
+        <v>14.019354294673825</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F48" s="19">
+        <f>(F47+F46)/F34*100</f>
+        <v>1.204</v>
+      </c>
+      <c r="G48" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="17">
+        <f>B26/B47</f>
+        <v>2.051182298026097</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="17">
+        <f>B33+B41</f>
+        <v>137.22117682976457</v>
+      </c>
+      <c r="B50" s="17">
+        <f>B35+B43</f>
+        <v>11.352765363049189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" t="s">
         <v>154</v>
-      </c>
-      <c r="D1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -17950,19 +19343,18 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4">
-        <f>B3+B2</f>
-        <v>13460</v>
+        <v>190</v>
+      </c>
+      <c r="B4" s="14">
+        <v>15000</v>
       </c>
       <c r="C4">
         <f>1/3*B4</f>
-        <v>4486.6666666666661</v>
+        <v>5000</v>
       </c>
       <c r="D4">
         <f>B4-C4</f>
-        <v>8973.3333333333339</v>
+        <v>10000</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -17974,19 +19366,19 @@
       </c>
       <c r="B5">
         <f>B4*3600*1000/(365.25*86400)</f>
-        <v>1535.4779831165868</v>
+        <v>1711.1567419575633</v>
       </c>
       <c r="C5">
         <f>C4*3600000/((1/3*365.25)*86400)</f>
-        <v>1535.4779831165865</v>
+        <v>1711.1567419575633</v>
       </c>
       <c r="D5" s="5">
         <f>D4*3600000/((2/3*365.25)*86400)</f>
-        <v>1535.477983116587</v>
+        <v>1711.1567419575633</v>
       </c>
       <c r="E5">
         <f>(C5+D5)/2</f>
-        <v>1535.4779831165868</v>
+        <v>1711.1567419575633</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -17995,7 +19387,7 @@
       </c>
       <c r="B6" s="3">
         <f>B5*(1-1/3.4)</f>
-        <v>1083.8668116117083</v>
+        <v>1207.8753472641622</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -18004,32 +19396,32 @@
       </c>
       <c r="B7" s="12">
         <f>B6*365.25*86400</f>
-        <v>34204235294.117645</v>
+        <v>38117647058.823524</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="12">
         <f>B7*30</f>
-        <v>1026127058823.5293</v>
+        <v>1143529411764.7058</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B11" s="5">
         <v>70</v>
@@ -18043,7 +19435,7 @@
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B12" s="5">
         <v>40</v>
@@ -18057,7 +19449,7 @@
     </row>
     <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B13" s="5">
         <f>B12+0.1*B12</f>
@@ -18073,7 +19465,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14">
         <f>B13*B11</f>
@@ -18089,7 +19481,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B15">
         <f>9+0.031*50</f>
@@ -18102,7 +19494,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B16">
         <f>B15-9</f>
@@ -18134,17 +19526,17 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -18152,8 +19544,8 @@
         <v>90</v>
       </c>
       <c r="B22">
-        <f>0.068*70</f>
-        <v>4.7600000000000007</v>
+        <f>0.063*73</f>
+        <v>4.5990000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -18170,16 +19562,16 @@
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B24" s="5">
         <f>1000-B23-B22</f>
-        <v>102.52503155592431</v>
+        <v>102.68603155592432</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B25">
         <f>0.012*70</f>
@@ -18188,7 +19580,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B26">
         <f>0.09*70</f>
@@ -18197,42 +19589,54 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f>1000-220</f>
+        <v>780</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f>A40/(40*30)</f>
+        <v>0.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>